<commit_message>
file 5 updated new
</commit_message>
<xml_diff>
--- a/5.xlsx
+++ b/5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="1" r:id="rId1"/>
@@ -550,15 +550,6 @@
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,22 +558,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -595,16 +582,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,16 +664,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>18251</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>172767</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>338913</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>172744</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>15063</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>39394</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -683,7 +683,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -696,8 +696,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11600651" y="3248025"/>
-          <a:ext cx="5807062" cy="3030244"/>
+          <a:off x="7716567" y="0"/>
+          <a:ext cx="4109496" cy="2144419"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,858 +998,826 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="8" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>44</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <v>66</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="3">
         <v>76</v>
       </c>
-      <c r="F10" s="6" t="str">
+      <c r="F10" s="3" t="str">
         <f>IF(C10+D10+E10&gt;180, "YES", "NO")</f>
         <v>YES</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>55</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>57</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="3">
         <v>78</v>
       </c>
-      <c r="F11" s="6" t="str">
+      <c r="F11" s="3" t="str">
         <f t="shared" ref="F11:F13" si="0">IF(C11+D11+E11&gt;200, "YES", "NO")</f>
         <v>NO</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>65</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>46</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="3">
         <v>57</v>
       </c>
-      <c r="F12" s="6" t="str">
+      <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>45</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>67</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="3">
         <v>64</v>
       </c>
-      <c r="F13" s="6" t="str">
+      <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="H14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="H16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="17" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="17" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="17" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="17" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="17" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="17" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="17" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="17" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="17" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="17" t="s">
+      <c r="A33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="A34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="17" t="s">
+      <c r="A38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="17" t="s">
+      <c r="A39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="17" t="s">
+      <c r="A40" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="17" t="s">
+      <c r="A41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="17" t="s">
+      <c r="A42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="17" t="s">
+      <c r="A43" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="17" t="s">
+      <c r="A44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="Q45" s="20"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="Q45" s="6"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="17" t="s">
+      <c r="A48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="17" t="s">
+      <c r="A50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="17" t="s">
+      <c r="A51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="17" t="s">
+      <c r="A52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="17" t="s">
+      <c r="A53" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C52:J52"/>
-    <mergeCell ref="C53:J53"/>
-    <mergeCell ref="C45:J45"/>
-    <mergeCell ref="C46:J46"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C48:J48"/>
-    <mergeCell ref="C49:J49"/>
-    <mergeCell ref="C51:J51"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C34:J34"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="C36:J36"/>
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="C38:J38"/>
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="H8:N9"/>
-    <mergeCell ref="H10:N11"/>
-    <mergeCell ref="B16:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:J2"/>
@@ -1859,6 +1827,42 @@
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H14:N15"/>
+    <mergeCell ref="H16:N17"/>
+    <mergeCell ref="B16:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C36:J36"/>
+    <mergeCell ref="C37:J37"/>
+    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C45:J45"/>
+    <mergeCell ref="C46:J46"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="C49:J49"/>
+    <mergeCell ref="C51:J51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>